<commit_message>
ClauseRef - WorkInProgress - Section header not styled when clauseref
</commit_message>
<xml_diff>
--- a/generated/latest_report_new.xlsx
+++ b/generated/latest_report_new.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="160">
   <si>
     <t>Allen &amp; Overy</t>
   </si>
@@ -30,7 +30,7 @@
     <t>The below loan portfolio report has been created by Allen &amp; Overy LLP.</t>
   </si>
   <si>
-    <t>This loan portfolio report is intended to classify portfolio loans and assist agency teams in ongoing loan management. It summarises certain key terms of the documentation as at 16:26 on 25/01/2017, but is not a substitute for the documentation itself. It does not constitute legal advice and should not be relied upon in relation to any amendment, waiver, dispute or other transaction relating to the underlying loan and neither Allen &amp; Overy LLP nor any other member of the A&amp;O group is liable for any loss arising from such use or reliance.</t>
+    <t>This loan portfolio report is intended to classify portfolio loans and assist agency teams in ongoing loan management. It summarises certain key terms of the documentation as at 17:11 on 25/01/2017, but is not a substitute for the documentation itself. It does not constitute legal advice and should not be relied upon in relation to any amendment, waiver, dispute or other transaction relating to the underlying loan and neither Allen &amp; Overy LLP nor any other member of the A&amp;O group is liable for any loss arising from such use or reliance.</t>
   </si>
   <si>
     <t>If you require any further information, please contact one of the people listed in section 1.5 of this report or your usual A&amp;O contact.</t>
@@ -108,6 +108,9 @@
     <t>Facilities</t>
   </si>
   <si>
+    <t xml:space="preserve">Clause Ref </t>
+  </si>
+  <si>
     <t>Total Commitments</t>
   </si>
   <si>
@@ -532,7 +535,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,8 +733,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -923,6 +937,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6EAEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1084,7 +1104,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1122,6 +1142,12 @@
     </xf>
     <xf numFmtId="14" fontId="25" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="25" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1481,7 +1507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G160"/>
+  <dimension ref="A1:H166"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1490,9 +1516,10 @@
     <col min="1" max="2" width="35.3671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.41796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.05078125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.83984375" customWidth="1"/>
     <col min="7" max="7" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.7" x14ac:dyDescent="0.55000000000000004">
@@ -1587,7 +1614,7 @@
       </c>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12">
         <v>1.4</v>
       </c>
@@ -1601,7 +1628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="8" t="s">
@@ -1611,7 +1638,7 @@
         <v>42748</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6">
         <v>1.5</v>
       </c>
@@ -1623,10 +1650,10 @@
       </c>
       <c r="D19" s="12"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5"/>
     </row>
-    <row r="21" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
@@ -1637,1578 +1664,1752 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="12">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="12">
         <v>2.1</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="8">
-        <v>100000</v>
-      </c>
-      <c r="G23" s="9">
-        <v>42766</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="F24" s="8">
+        <v>100000</v>
+      </c>
+      <c r="G24" s="9">
+        <v>42766</v>
+      </c>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="8">
+      <c r="E25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="8">
         <v>900000</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G25" s="9">
         <v>117640</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="6">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="B26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6">
-        <v>2.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="8">
+      <c r="D31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="6">
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="6">
         <v>2.7</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="6">
-        <v>2.8</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="12"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="8">
+        <v>2000</v>
+      </c>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="6">
-        <v>2.1</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="8">
+      <c r="D39" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="8">
         <v>3000</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="6">
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="6">
         <v>2.11</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="6"/>
       <c r="B41" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6"/>
       <c r="B42" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="6"/>
       <c r="B44" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="6">
-        <v>2.12</v>
-      </c>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="6">
-        <v>2.13</v>
+        <v>2.12</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="6">
-        <v>2.14</v>
+        <v>2.13</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="6">
+        <v>2.14</v>
+      </c>
       <c r="B48" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="6"/>
       <c r="B50" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="6"/>
       <c r="B51" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="6"/>
       <c r="B52" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="6"/>
       <c r="B53" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="6"/>
       <c r="B54" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12" t="s">
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="8">
+      <c r="D56" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H56" s="12"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="8">
         <v>12</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D57" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H57" s="12"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="12"/>
+      <c r="B59" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6" t="s">
+      <c r="H59" s="12"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="8">
+        <v>6</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58" s="7" t="s">
+      <c r="H60" s="12"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="8">
-        <v>6</v>
-      </c>
-      <c r="D59" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="7" t="s">
+      <c r="H62" s="12"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="8">
+        <v>3</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H63" s="12"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="8">
-        <v>3</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6" t="s">
+      <c r="D65" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H65" s="12"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="8">
+        <v>1</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="7" t="s">
+      <c r="H66" s="12"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="8">
-        <v>1</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="8">
+      <c r="D68" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H68" s="12"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="8">
         <v>2</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="D69" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C69" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H69" s="12"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="6"/>
       <c r="B70" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="6"/>
       <c r="B71" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="6">
-        <v>2.15</v>
-      </c>
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="6"/>
       <c r="B72" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="6">
-        <v>2.16</v>
+        <v>2.15</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="6">
-        <v>2.17</v>
+        <v>2.16</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>78</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="12">
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="6">
+        <v>2.17</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="12">
         <v>2.1800000000000002</v>
       </c>
-      <c r="B75" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D75" s="7" t="s">
+      <c r="B76" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D76" s="8">
+      <c r="D76" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H76" s="12"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" s="8">
         <v>5000</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="6">
+      <c r="H77" s="12"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="6">
         <v>2.19</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="6">
-        <v>2.2000000000000002</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="6">
-        <v>2.21</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B79" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="5"/>
-    </row>
-    <row r="81" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="10" t="s">
+      <c r="H79" s="6"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="6">
+        <v>2.21</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="6">
+      <c r="C80" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="5"/>
+    </row>
+    <row r="82" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="15"/>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="6">
         <v>3.1</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C82" s="14">
+      <c r="B84" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84" s="16">
         <v>0.66666666666666674</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="6">
+      <c r="D84" s="6"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="6">
         <v>3.2</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="6">
+      <c r="B85" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D85" s="6"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="6">
         <v>3.3</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C84" s="6" t="s">
+      <c r="B86" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="6">
+      <c r="C86" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D86" s="6"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="6">
         <v>3.4</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="6">
+      <c r="B87" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="6"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="6">
         <v>3.5</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="5"/>
-    </row>
-    <row r="88" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="10" t="s">
+      <c r="B88" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="6">
+      <c r="C88" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D88" s="6"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="5"/>
+    </row>
+    <row r="90" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="15"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C89" s="6" t="s">
+      <c r="B92" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="6">
+      <c r="C92" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="6"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="6">
         <v>4.2</v>
       </c>
-      <c r="B90" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="6">
+      <c r="B93" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="6">
         <v>4.3</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="6">
+      <c r="B94" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D94" s="6"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C92" s="6" t="s">
+      <c r="B95" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="6">
+      <c r="C95" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="6">
         <v>4.5</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C93" s="6" t="s">
+      <c r="B96" s="6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="6">
+      <c r="C96" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="6">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B97" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D98" s="6"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="6">
+        <v>4.8</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="6">
-        <v>4.7</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="6">
-        <v>4.8</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="5"/>
-    </row>
-    <row r="98" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="6">
+      <c r="D99" s="6"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="5"/>
+    </row>
+    <row r="101" spans="1:5" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B99" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="6">
+      <c r="B102" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="6">
         <v>5.2</v>
       </c>
-      <c r="B100" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C100" s="6" t="s">
+      <c r="B103" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="6">
+      <c r="C103" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="6">
         <v>5.3</v>
       </c>
-      <c r="B101" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C101" s="6" t="s">
+      <c r="B104" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="6">
+      <c r="C104" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="6">
         <v>5.4</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="6">
+      <c r="B105" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="6">
         <v>5.5</v>
       </c>
-      <c r="B103" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="6">
+      <c r="B106" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="6">
         <v>5.6</v>
       </c>
-      <c r="B104" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="5"/>
-    </row>
-    <row r="106" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="10" t="s">
+      <c r="B107" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B106" s="10"/>
-      <c r="C106" s="10"/>
-      <c r="D106" s="10"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="6">
+      <c r="C107" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="5"/>
+    </row>
+    <row r="109" spans="1:5" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="15"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="15"/>
+      <c r="D110" s="15"/>
+      <c r="E110" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="6">
         <v>6.1</v>
       </c>
-      <c r="B107" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="6"/>
-      <c r="B108" s="6" t="s">
+      <c r="B111" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D108" s="12"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="6"/>
-      <c r="B109" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D109" s="12"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="6"/>
-      <c r="B110" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C110" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D110" s="12"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="6"/>
-      <c r="B111" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>117</v>
-      </c>
+      <c r="C111" s="12"/>
       <c r="D111" s="12"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E111" s="6"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="6"/>
       <c r="B112" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D112" s="12"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E112" s="6"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="6"/>
       <c r="B113" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D113" s="12"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E113" s="6"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="6"/>
       <c r="B114" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="D114" s="12"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="6">
-        <v>6.2</v>
-      </c>
+      <c r="E114" s="6"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="6"/>
       <c r="B115" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C115" s="12"/>
+        <v>121</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>118</v>
+      </c>
       <c r="D115" s="12"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="6"/>
       <c r="B116" s="6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D116" s="12"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="6"/>
       <c r="B117" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C117" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C117" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="D117" s="12"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="6"/>
       <c r="B118" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="D118" s="12"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="6"/>
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="6">
+        <v>6.2</v>
+      </c>
       <c r="B119" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>117</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C119" s="12"/>
       <c r="D119" s="12"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="6"/>
       <c r="B120" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D120" s="12"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="6"/>
       <c r="B121" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D121" s="12"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="6"/>
       <c r="B122" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D122" s="12"/>
+      <c r="E122" s="6"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="6"/>
+      <c r="B123" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D123" s="12"/>
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="6"/>
+      <c r="B124" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C124" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D124" s="12"/>
+      <c r="E124" s="6"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="6"/>
+      <c r="B125" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C122" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D122" s="12"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="6">
+      <c r="C125" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D125" s="12"/>
+      <c r="E125" s="6"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="6"/>
+      <c r="B126" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D126" s="12"/>
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="6">
         <v>6.3</v>
       </c>
-      <c r="B123" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D123" s="12"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="6">
+      <c r="B127" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C127" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D127" s="12"/>
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="6">
         <v>6.4</v>
       </c>
-      <c r="B124" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C124" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D124" s="12"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="6">
+      <c r="B128" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D128" s="12"/>
+      <c r="E128" s="6"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="6">
         <v>6.5</v>
       </c>
-      <c r="B125" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C125" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D125" s="12"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="6">
+      <c r="B129" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129" s="12"/>
+      <c r="E129" s="6"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="6">
         <v>6.6</v>
       </c>
-      <c r="B126" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C126" s="12" t="s">
+      <c r="B130" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D126" s="12"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="12">
+      <c r="C130" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D130" s="12"/>
+      <c r="E130" s="6"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="12">
         <v>6.7</v>
       </c>
-      <c r="B127" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D127" s="7" t="s">
+      <c r="B131" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C131" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="12"/>
-      <c r="B128" s="12"/>
-      <c r="C128" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D128" s="8">
+      <c r="D131" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E131" s="12"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="12"/>
+      <c r="B132" s="12"/>
+      <c r="C132" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D132" s="8">
         <v>5000</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="6">
+      <c r="E132" s="12"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="6">
         <v>6.8</v>
       </c>
-      <c r="B129" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C129" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D129" s="12"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="5"/>
-    </row>
-    <row r="131" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="10" t="s">
+      <c r="B133" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B131" s="10"/>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="6">
+      <c r="C133" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D133" s="12"/>
+      <c r="E133" s="6"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="5"/>
+    </row>
+    <row r="135" spans="1:5" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B135" s="10"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="15"/>
+      <c r="B136" s="15"/>
+      <c r="C136" s="15"/>
+      <c r="D136" s="15"/>
+      <c r="E136" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="6">
         <v>7.1</v>
       </c>
-      <c r="B132" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C132" s="12" t="s">
+      <c r="B137" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D132" s="12"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="6">
+      <c r="C137" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D137" s="12"/>
+      <c r="E137" s="6"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="6">
         <v>7.2</v>
       </c>
-      <c r="B133" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C133" s="12"/>
-      <c r="D133" s="12"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="6"/>
-      <c r="B134" s="6"/>
-      <c r="C134" s="12" t="s">
+      <c r="B138" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D134" s="12"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="12">
+      <c r="C138" s="12"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="6"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="6"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D139" s="12"/>
+      <c r="E139" s="6"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="12">
         <v>7.3</v>
       </c>
-      <c r="B135" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C135" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D135" s="7" t="s">
+      <c r="B140" s="12" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="12"/>
-      <c r="B136" s="12"/>
-      <c r="C136" s="8">
+      <c r="C140" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E140" s="12"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="12"/>
+      <c r="B141" s="12"/>
+      <c r="C141" s="8">
         <v>3</v>
       </c>
-      <c r="D136" s="8" t="s">
+      <c r="D141" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E141" s="12"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="12">
+        <v>7.4</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D142" s="7" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="12">
-        <v>7.4</v>
-      </c>
-      <c r="B137" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D137" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="12"/>
-      <c r="B138" s="12"/>
-      <c r="C138" s="8">
+      <c r="E142" s="12"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="12"/>
+      <c r="B143" s="12"/>
+      <c r="C143" s="8">
         <v>12</v>
       </c>
-      <c r="D138" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="12">
+      <c r="D143" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E143" s="12"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="12">
         <v>7.5</v>
       </c>
-      <c r="B139" s="12" t="s">
+      <c r="B144" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E144" s="12"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="12"/>
+      <c r="B145" s="12"/>
+      <c r="C145" s="8">
+        <v>10</v>
+      </c>
+      <c r="D145" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C139" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D139" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
-      <c r="C140" s="8">
-        <v>10</v>
-      </c>
-      <c r="D140" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="12">
+      <c r="E145" s="12"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="12">
         <v>7.6</v>
       </c>
-      <c r="B141" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D141" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
-      <c r="C142" s="8">
+      <c r="B146" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D146" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E146" s="12"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="12"/>
+      <c r="B147" s="12"/>
+      <c r="C147" s="8">
         <v>5</v>
       </c>
-      <c r="D142" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="5"/>
-    </row>
-    <row r="144" spans="1:4" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="B144" s="10"/>
-      <c r="C144" s="10"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="6">
+      <c r="D147" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E147" s="12"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="5"/>
+    </row>
+    <row r="149" spans="1:5" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="15"/>
+      <c r="B150" s="15"/>
+      <c r="C150" s="15"/>
+      <c r="D150" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" s="6">
         <v>8.1</v>
       </c>
-      <c r="B145" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="C145" s="6">
+      <c r="B151" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C151" s="6">
         <v>12</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="6">
+      <c r="D151" s="6"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" s="6">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B146" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C146" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" s="6">
+      <c r="B152" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D152" s="6"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" s="6">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B147" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C147" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" s="6">
+      <c r="B153" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D153" s="6"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="6">
         <v>8.4</v>
       </c>
-      <c r="B148" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C148" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" s="5"/>
-    </row>
-    <row r="150" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A150" s="10" t="s">
+      <c r="B154" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B150" s="10"/>
-      <c r="C150" s="10"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A151" s="6">
+      <c r="C154" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D154" s="6"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="5"/>
+    </row>
+    <row r="156" spans="1:5" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" s="10"/>
+      <c r="C156" s="10"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="6">
         <v>9.1</v>
       </c>
-      <c r="B151" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A152" s="6">
+      <c r="B157" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C157" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="6">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B152" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C152" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A153" s="5"/>
-    </row>
-    <row r="154" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A154" s="10" t="s">
+      <c r="B158" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B154" s="10"/>
-      <c r="C154" s="10"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A155" s="6">
+      <c r="C158" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="5"/>
+    </row>
+    <row r="160" spans="1:5" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B160" s="10"/>
+      <c r="C160" s="10"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" s="6">
         <v>10.1</v>
       </c>
-      <c r="B155" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C155" s="6" t="s">
+      <c r="B161" s="6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A156" s="5"/>
-    </row>
-    <row r="157" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A157" s="10" t="s">
+      <c r="C161" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B157" s="10"/>
-      <c r="C157" s="10"/>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A158" s="6">
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="5"/>
+    </row>
+    <row r="163" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="6">
         <v>11.1</v>
       </c>
-      <c r="B158" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C158" s="6" t="s">
+      <c r="B164" s="6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A159" s="6">
+      <c r="C164" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="6">
         <v>11.2</v>
       </c>
-      <c r="B159" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C159" s="6">
+      <c r="B165" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C165" s="6">
         <v>123</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A160" s="5"/>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="A144:C144"/>
+  <mergeCells count="129">
+    <mergeCell ref="A160:C160"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="A149:C149"/>
     <mergeCell ref="A150:C150"/>
-    <mergeCell ref="A154:C154"/>
-    <mergeCell ref="A157:C157"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="B137:B138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="B139:B140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="B141:B142"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="A156:C156"/>
+    <mergeCell ref="E140:E141"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="E144:E145"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="A131:A132"/>
+    <mergeCell ref="B131:B132"/>
+    <mergeCell ref="E131:E132"/>
     <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="B135:B136"/>
+    <mergeCell ref="A135:D135"/>
     <mergeCell ref="C124:D124"/>
     <mergeCell ref="C125:D125"/>
     <mergeCell ref="C126:D126"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="B127:B128"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
     <mergeCell ref="C129:D129"/>
     <mergeCell ref="C118:D118"/>
     <mergeCell ref="C119:D119"/>
@@ -3222,74 +3423,84 @@
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="C116:D116"/>
     <mergeCell ref="C117:D117"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A110:D110"/>
     <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="H76:H77"/>
     <mergeCell ref="C78:G78"/>
     <mergeCell ref="C79:G79"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A83:C83"/>
     <mergeCell ref="C72:G72"/>
     <mergeCell ref="C73:G73"/>
     <mergeCell ref="C74:G74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C66:G66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C67:G67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C61:G61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="C64:G64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="H65:H66"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="C53:G53"/>
     <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
     <mergeCell ref="C46:G46"/>
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="H39:H40"/>
     <mergeCell ref="C41:G41"/>
     <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="H31:H32"/>
     <mergeCell ref="C33:G33"/>
     <mergeCell ref="C34:G34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="C29:G29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="H23:H25"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>

</xml_diff>